<commit_message>
a lot of small changes
</commit_message>
<xml_diff>
--- a/01_DATA/BB22_plant_sugar_data.xlsx
+++ b/01_DATA/BB22_plant_sugar_data.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simo/Library/CloudStorage/GoogleDrive-simo1996s@gmail.com/My Drive/ETH/Master Thesis/Bumblebee_2022/01_DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1105C5-36B3-FA4D-A674-CD436EF971FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461CF199-2180-3749-8766-987F165D2228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sugar" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sugar!$A$1:$C$98</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1175,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2263,6 +2266,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C98" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C98">
     <sortCondition ref="A7:A98"/>
   </sortState>

</xml_diff>